<commit_message>
LEAP-75 Update Add SAPCND + SAPCN
</commit_message>
<xml_diff>
--- a/Treeview_Compartiments_dev_sapco.xlsx
+++ b/Treeview_Compartiments_dev_sapco.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://agropur-my.sharepoint.com/personal/cesar_arce_agropur_com/Documents/Documents/Python Scripts/AWS_S3_Glue_Dev_manual_commit_gzipfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="8_{5F1195FD-7DD5-425A-BB16-96E5C38AD771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5869DB37-768A-4F79-BC50-091E6F78AB49}"/>
+  <xr:revisionPtr revIDLastSave="123" documentId="8_{5F1195FD-7DD5-425A-BB16-96E5C38AD771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CDD290D-773D-435F-AA09-820112B408EF}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2850" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{47CDF58C-05E4-437B-B922-21426A76DED4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2331" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2345" uniqueCount="248">
   <si>
     <t>source</t>
   </si>
@@ -775,6 +775,12 @@
   </si>
   <si>
     <t>Level_7</t>
+  </si>
+  <si>
+    <t>SAPCND_CONDINDX/</t>
+  </si>
+  <si>
+    <t>SAPCN/</t>
   </si>
 </sst>
 </file>
@@ -1150,18 +1156,18 @@
       <selection activeCell="A183" sqref="A183"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="69.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.453125" customWidth="1"/>
+    <col min="1" max="1" width="70.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1190,7 +1196,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>CONCATENATE(C2,D2,E2,F2,G2,H2)</f>
         <v>/SAPCO/Inbound/Financials/Costing/</v>
@@ -1215,7 +1221,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A68" si="0">CONCATENATE(C3,D3,E3,F3,G3,H3)</f>
         <v>/SAPCO/Inbound/Financials/Profitability/</v>
@@ -1240,7 +1246,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/Financials/Profitability/Historical/</v>
@@ -1268,7 +1274,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/Financials/Profitability/ZIPRFANLZFINLCUB/</v>
@@ -1296,7 +1302,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/Inventory/Balances/</v>
@@ -1321,7 +1327,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/Inventory/Balances/ZISCINVBALFINALC/</v>
@@ -1349,7 +1355,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/Inventory/Transactions/</v>
@@ -1374,7 +1380,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/Manufacturing/Overview/</v>
@@ -1399,7 +1405,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/Manufacturing/Process Quality/</v>
@@ -1424,7 +1430,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/Procurement and Spend/Invoice Lines/</v>
@@ -1449,7 +1455,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/Procurement and Spend/Purchase Orders/</v>
@@ -1474,7 +1480,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/Procurement and Spend/Purchase Receipts/</v>
@@ -1499,7 +1505,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/Sales/Invoice Lines/</v>
@@ -1524,7 +1530,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/Sales/Order Lines/</v>
@@ -1549,7 +1555,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/Sales/Ship Lines/</v>
@@ -1574,7 +1580,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/Sales/test_TOBEDELETED/</v>
@@ -1599,7 +1605,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/FIN/FIN_T001/</v>
@@ -1627,7 +1633,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/FIN/T001/</v>
@@ -1655,7 +1661,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/A526/</v>
@@ -1683,7 +1689,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/A528/</v>
@@ -1711,7 +1717,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/A531/</v>
@@ -1739,7 +1745,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/A532/</v>
@@ -1767,7 +1773,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/A533/</v>
@@ -1795,7 +1801,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/A534/</v>
@@ -1823,7 +1829,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/A537/</v>
@@ -1851,7 +1857,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/A541/</v>
@@ -1879,7 +1885,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/A542/</v>
@@ -1907,7 +1913,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/A701/</v>
@@ -1935,7 +1941,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/A702/</v>
@@ -1963,7 +1969,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/A703/</v>
@@ -1991,7 +1997,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/ADR2/</v>
@@ -2019,7 +2025,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/ADR6/</v>
@@ -2047,7 +2053,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/ADRC/</v>
@@ -2075,7 +2081,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/AUSP/</v>
@@ -2103,7 +2109,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/B501/</v>
@@ -2131,7 +2137,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/B503/</v>
@@ -2159,7 +2165,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/B504/</v>
@@ -2187,7 +2193,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/B511/</v>
@@ -2215,7 +2221,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/B512/</v>
@@ -2243,7 +2249,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/BUT000/</v>
@@ -2271,7 +2277,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/BUT020/</v>
@@ -2299,7 +2305,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/BUT100/</v>
@@ -2327,7 +2333,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/DFKKBPTAXNUM/</v>
@@ -2355,7 +2361,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/EDIPHONE/</v>
@@ -2383,7 +2389,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/EDP12/</v>
@@ -2411,7 +2417,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/EDP13/</v>
@@ -2439,7 +2445,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/EDP21/</v>
@@ -2467,7 +2473,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/EDPAR/</v>
@@ -2495,7 +2501,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/EDPP1/</v>
@@ -2523,7 +2529,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/EDSDC/</v>
@@ -2551,7 +2557,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KNA1/</v>
@@ -2579,7 +2585,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KNB1/</v>
@@ -2607,7 +2613,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KNB5/</v>
@@ -2635,7 +2641,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KNMT/</v>
@@ -2663,7 +2669,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KNMTA/</v>
@@ -2691,7 +2697,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KNVH/</v>
@@ -2719,7 +2725,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KNVI/</v>
@@ -2747,7 +2753,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KNVP/</v>
@@ -2775,7 +2781,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KNVV/</v>
@@ -2803,7 +2809,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KONDH/</v>
@@ -2831,7 +2837,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KONH/</v>
@@ -2859,7 +2865,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KONM/</v>
@@ -2887,7 +2893,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KONP/</v>
@@ -2915,7 +2921,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KOTH001/</v>
@@ -2943,7 +2949,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KOTH900/</v>
@@ -2971,7 +2977,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KOTH903/</v>
@@ -2999,7 +3005,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/NACH/</v>
@@ -3027,7 +3033,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f t="shared" ref="A69:A132" si="2">CONCATENATE(C69,D69,E69,F69,G69,H69)</f>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/STXH/</v>
@@ -3055,7 +3061,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/STXL/</v>
@@ -3083,7 +3089,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/TVKO/</v>
@@ -3111,7 +3117,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/UDMBPPROFILE/</v>
@@ -3139,7 +3145,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/UDMBPSEGMENTS/</v>
@@ -3167,7 +3173,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/UKMBP/</v>
@@ -3195,7 +3201,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/ZTCO/</v>
@@ -3223,7 +3229,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/AFPO/</v>
@@ -3251,7 +3257,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/AUFK/</v>
@@ -3279,7 +3285,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/CABN/</v>
@@ -3307,7 +3313,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/CAUFV/</v>
@@ -3335,7 +3341,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/CRCA/</v>
@@ -3363,7 +3369,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/CRCO/</v>
@@ -3391,7 +3397,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/CRHD/</v>
@@ -3419,7 +3425,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/CRTX/</v>
@@ -3447,7 +3453,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/KAKO/</v>
@@ -3475,7 +3481,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/KAKT/</v>
@@ -3503,7 +3509,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/KLAH/</v>
@@ -3531,7 +3537,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/MAKT/</v>
@@ -3559,7 +3565,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/MAPL/</v>
@@ -3587,7 +3593,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/MARA/</v>
@@ -3615,7 +3621,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/MARC/</v>
@@ -3643,7 +3649,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/MARD/</v>
@@ -3671,7 +3677,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/MARM/</v>
@@ -3699,7 +3705,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/MAST/</v>
@@ -3727,7 +3733,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/MKAL/</v>
@@ -3755,7 +3761,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/MLAN/</v>
@@ -3783,7 +3789,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/MVKE/</v>
@@ -3811,7 +3817,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/PLKO/</v>
@@ -3839,7 +3845,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/PLMK/</v>
@@ -3867,7 +3873,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/PLPO/</v>
@@ -3895,7 +3901,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/QCVK/</v>
@@ -3923,7 +3929,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/QCVM/</v>
@@ -3951,7 +3957,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/QCVMT/</v>
@@ -3979,7 +3985,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/QCVV/</v>
@@ -4007,7 +4013,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/QMAT/</v>
@@ -4035,7 +4041,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/QMTB/</v>
@@ -4063,7 +4069,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/QMTT/</v>
@@ -4091,7 +4097,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/QPMK/</v>
@@ -4119,7 +4125,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/QPMZ/</v>
@@ -4147,7 +4153,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/RESB/</v>
@@ -4175,7 +4181,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/SAPAPO/</v>
@@ -4203,7 +4209,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/STKO/</v>
@@ -4231,7 +4237,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/STPO/</v>
@@ -4259,7 +4265,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/TCRCOT/</v>
@@ -4287,7 +4293,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/A017/</v>
@@ -4315,7 +4321,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/A018/</v>
@@ -4343,7 +4349,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/EINA/</v>
@@ -4371,7 +4377,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/EINE/</v>
@@ -4399,7 +4405,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/EORD/</v>
@@ -4427,7 +4433,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/KNBK/</v>
@@ -4455,7 +4461,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/LFA1/</v>
@@ -4483,7 +4489,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/LFB1/</v>
@@ -4511,7 +4517,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/LFBK/</v>
@@ -4539,7 +4545,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/LFBW/</v>
@@ -4567,7 +4573,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/LFM1/</v>
@@ -4595,7 +4601,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/T001W/</v>
@@ -4623,7 +4629,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/T024E/</v>
@@ -4651,7 +4657,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/WYT3/</v>
@@ -4679,7 +4685,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/ANEP/</v>
@@ -4707,7 +4713,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/ANLA/</v>
@@ -4735,7 +4741,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/ANLB/</v>
@@ -4763,7 +4769,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/ANLC/</v>
@@ -4791,7 +4797,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" t="str">
         <f t="shared" si="2"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/ANLH/</v>
@@ -4819,7 +4825,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" t="str">
         <f t="shared" ref="A133:A190" si="4">CONCATENATE(C133,D133,E133,F133,G133,H133)</f>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/ANLZ/</v>
@@ -4847,7 +4853,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/BKPF/</v>
@@ -4875,7 +4881,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/BNKA/</v>
@@ -4903,7 +4909,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/BSET/</v>
@@ -4931,7 +4937,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/BSIS/</v>
@@ -4959,7 +4965,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/CSKS/</v>
@@ -4987,7 +4993,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/CSKT/</v>
@@ -5015,7 +5021,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/PRHI/</v>
@@ -5043,7 +5049,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/PROJ/</v>
@@ -5071,7 +5077,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/PRPS/</v>
@@ -5099,7 +5105,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/SKA1/</v>
@@ -5127,7 +5133,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/SKAT/</v>
@@ -5155,7 +5161,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/SKB1/</v>
@@ -5183,7 +5189,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/ZBSEG/</v>
@@ -5211,7 +5217,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/ZBSIK/</v>
@@ -5239,7 +5245,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/AQUA/</v>
@@ -5267,7 +5273,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/BINMAT/</v>
@@ -5295,7 +5301,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/CONDINDX/</v>
@@ -5323,7 +5329,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/HUHDR/</v>
@@ -5351,7 +5357,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/LAGP/</v>
@@ -5379,7 +5385,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/MATLWH/</v>
@@ -5407,7 +5413,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/MATLWHST/</v>
@@ -5435,7 +5441,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/MCHA/</v>
@@ -5463,7 +5469,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/MKPF/</v>
@@ -5491,7 +5497,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/MSEG/</v>
@@ -5519,7 +5525,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/PAPAK/</v>
@@ -5547,7 +5553,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/PNPAKH/</v>
@@ -5575,7 +5581,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/PVPAKC/</v>
@@ -5603,7 +5609,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/PVPAKL/</v>
@@ -5631,7 +5637,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/QUAN/</v>
@@ -5659,7 +5665,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SAPAPO/SAPAPO_MATLWH/</v>
@@ -5690,7 +5696,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SAPAPO/SAPAPO_MATLWHST/</v>
@@ -5721,7 +5727,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SAPAPO/SAPAPO_TR/</v>
@@ -5752,7 +5758,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SAPAPO/SAPAPO_TRM/</v>
@@ -5783,7 +5789,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SAPAPO/SAPAPO_TRMC/</v>
@@ -5814,7 +5820,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SAPAPO/SAPAPO_TRMCARR/</v>
@@ -5845,7 +5851,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SAPCND/</v>
@@ -5873,7 +5879,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCMB/SCMB_TOENTITY/</v>
@@ -5904,7 +5910,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCMB/SCMB_ZONE_D/</v>
@@ -5935,7 +5941,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCMB/SCMB_ZONE_P/</v>
@@ -5966,7 +5972,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCMB/SCMB_ZONE_R/</v>
@@ -5997,7 +6003,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCMB/SCMB_ZONE/</v>
@@ -6028,7 +6034,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/SCWM_AQUA/</v>
@@ -6059,7 +6065,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/SCWM_BINMAT/</v>
@@ -6090,7 +6096,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/SCWM_HUHDR/</v>
@@ -6121,7 +6127,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/SCWM_LAGP/</v>
@@ -6152,7 +6158,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/SCWM_PAPAK/</v>
@@ -6183,7 +6189,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/SCWM_PNPAKH/</v>
@@ -6214,7 +6220,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/SCWM_PVPAKC/</v>
@@ -6245,7 +6251,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/SCWM_PVPAKL/</v>
@@ -6276,7 +6282,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/SCWM_QUAN/</v>
@@ -6307,7 +6313,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/T001L/</v>
@@ -6335,7 +6341,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/TR/</v>
@@ -6363,7 +6369,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/TRM/</v>
@@ -6391,7 +6397,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/TRMC/</v>
@@ -6419,7 +6425,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/TRMCARR/</v>
@@ -6447,7 +6453,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/TVST</v>
@@ -6475,7 +6481,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/TEST/T001/</v>
@@ -6510,26 +6516,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796BCB69-F888-4B7E-92ED-E9FA4A26428F}">
-  <dimension ref="A1:K194"/>
+  <dimension ref="A1:K196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H107" sqref="H107"/>
+    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G174" sqref="G174"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="69.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1796875" customWidth="1"/>
-    <col min="8" max="8" width="10.54296875" customWidth="1"/>
-    <col min="9" max="9" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="70.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6561,7 +6567,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>CONCATENATE(C2,D2,E2,F2,G2,H2)</f>
         <v>/SAPCO/Inbound/FINANCIAL/COSTING/</v>
@@ -6586,7 +6592,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A68" si="0">CONCATENATE(C3,D3,E3,F3,G3,H3)</f>
         <v>/SAPCO/Inbound/FINANCIAL/PROFITABILITY/HISTORICAL/</v>
@@ -6614,7 +6620,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" ref="A4" si="1">CONCATENATE(C4,D4,E4,F4,G4,H4)</f>
         <v>/SAPCO/Inbound/FINANCIAL/PROFITABILITY/PROFITABILITY/</v>
@@ -6642,7 +6648,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/INVENTORY/BALANCES/</v>
@@ -6667,7 +6673,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/INVENTORY/TRANSACTIONS/</v>
@@ -6692,7 +6698,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MANUFACTURING/OVERVIEW/</v>
@@ -6717,7 +6723,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MANUFACTURING/PROCESSQUALITY/</v>
@@ -6742,7 +6748,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/PROCUREMENTANDSPEND/INVOICELINE/</v>
@@ -6767,7 +6773,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/PROCUREMENTANDSPEND/PURCHASEORDER/</v>
@@ -6792,7 +6798,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/PROCUREMENTANDSPEND/PURCHASERECEIPT/</v>
@@ -6817,7 +6823,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/SALE/INVOICELINES/</v>
@@ -6842,7 +6848,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/SALE/ORDERLINES/</v>
@@ -6867,7 +6873,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/SALE/SHIPLINES/</v>
@@ -6892,7 +6898,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/FIN/FIN_T001/</v>
@@ -6920,7 +6926,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/FIN/T001/</v>
@@ -6948,7 +6954,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="str">
         <f t="shared" ref="A17:A19" si="4">CONCATENATE(C17,D17,E17,F17,G17,H17)</f>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/FIN/T009/</v>
@@ -6979,7 +6985,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/FIN/T009B/</v>
@@ -7010,7 +7016,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="str">
         <f t="shared" si="4"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/FIN/T009C/</v>
@@ -7041,7 +7047,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/A526/</v>
@@ -7069,7 +7075,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/A528/</v>
@@ -7097,7 +7103,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/A531/</v>
@@ -7125,7 +7131,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/A532/</v>
@@ -7153,7 +7159,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/A533/</v>
@@ -7181,7 +7187,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/A534/</v>
@@ -7209,7 +7215,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/A537/</v>
@@ -7237,7 +7243,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/A541/</v>
@@ -7265,7 +7271,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/A542/</v>
@@ -7293,7 +7299,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/A701/</v>
@@ -7321,7 +7327,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/A702/</v>
@@ -7349,7 +7355,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/A703/</v>
@@ -7377,7 +7383,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/ADR2/</v>
@@ -7405,7 +7411,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/ADR6/</v>
@@ -7433,7 +7439,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/ADRC/</v>
@@ -7461,7 +7467,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/AUSP/</v>
@@ -7489,7 +7495,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/B501/</v>
@@ -7517,7 +7523,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/B503/</v>
@@ -7545,7 +7551,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/B504/</v>
@@ -7573,7 +7579,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/B511/</v>
@@ -7601,7 +7607,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/B512/</v>
@@ -7629,7 +7635,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/BUT000/</v>
@@ -7657,7 +7663,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/BUT020/</v>
@@ -7685,7 +7691,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/BUT100/</v>
@@ -7713,7 +7719,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/DFKKBPTAXNUM/</v>
@@ -7741,7 +7747,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/EDIPHONE/</v>
@@ -7769,7 +7775,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/EDP12/</v>
@@ -7797,7 +7803,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/EDP13/</v>
@@ -7825,7 +7831,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/EDP21/</v>
@@ -7853,7 +7859,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/EDPAR/</v>
@@ -7881,7 +7887,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/EDPP1/</v>
@@ -7909,7 +7915,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/EDSDC/</v>
@@ -7937,7 +7943,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KNA1/</v>
@@ -7965,7 +7971,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KNB1/</v>
@@ -7993,7 +7999,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KNB5/</v>
@@ -8021,7 +8027,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KNMT/</v>
@@ -8049,7 +8055,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KNMTA/</v>
@@ -8077,7 +8083,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KNVH/</v>
@@ -8105,7 +8111,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KNVI/</v>
@@ -8133,7 +8139,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KNVP/</v>
@@ -8161,7 +8167,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KNVV/</v>
@@ -8189,7 +8195,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KONDH/</v>
@@ -8217,7 +8223,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KONH/</v>
@@ -8245,7 +8251,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KONM/</v>
@@ -8273,7 +8279,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KONP/</v>
@@ -8301,7 +8307,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KOTH001/</v>
@@ -8329,7 +8335,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KOTH900/</v>
@@ -8357,7 +8363,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/KOTH903/</v>
@@ -8385,7 +8391,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f t="shared" si="0"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/NACH/</v>
@@ -8413,7 +8419,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f t="shared" ref="A69:A136" si="8">CONCATENATE(C69,D69,E69,F69,G69,H69)</f>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/STXH/</v>
@@ -8441,7 +8447,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/STXL/</v>
@@ -8469,7 +8475,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="str">
         <f t="shared" ref="A71:A72" si="10">CONCATENATE(C71,D71,E71,F71,G71,H71)</f>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/T6821/</v>
@@ -8500,7 +8506,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="str">
         <f t="shared" si="10"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/T685/</v>
@@ -8531,7 +8537,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/TVKO/</v>
@@ -8559,7 +8565,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/UDMBPPROFILE/</v>
@@ -8587,7 +8593,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/UDMBPSEGMENTS/</v>
@@ -8615,7 +8621,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/UKMBP/</v>
@@ -8643,7 +8649,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/OTC/ZTCO/</v>
@@ -8671,7 +8677,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/AFPO/</v>
@@ -8699,7 +8705,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/AUFK/</v>
@@ -8727,7 +8733,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/CABN/</v>
@@ -8755,7 +8761,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/CAUFV/</v>
@@ -8783,7 +8789,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/CRCA/</v>
@@ -8811,7 +8817,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/CRCO/</v>
@@ -8839,7 +8845,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/CRHD/</v>
@@ -8867,7 +8873,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/CRTX/</v>
@@ -8895,7 +8901,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/KAKO/</v>
@@ -8923,7 +8929,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/KAKT/</v>
@@ -8951,7 +8957,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/KLAH/</v>
@@ -8979,7 +8985,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/MAKT/</v>
@@ -9007,7 +9013,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/MAPL/</v>
@@ -9035,7 +9041,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/MARA/</v>
@@ -9063,7 +9069,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/MARC/</v>
@@ -9091,7 +9097,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/MARD/</v>
@@ -9119,7 +9125,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/MARM/</v>
@@ -9147,7 +9153,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/MAST/</v>
@@ -9175,7 +9181,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/MKAL/</v>
@@ -9203,7 +9209,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/MLAN/</v>
@@ -9231,7 +9237,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/MVKE/</v>
@@ -9259,7 +9265,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/PLKO/</v>
@@ -9287,7 +9293,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/PLMK/</v>
@@ -9315,7 +9321,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/PLPO/</v>
@@ -9343,7 +9349,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/QCVK/</v>
@@ -9371,7 +9377,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/QCVM/</v>
@@ -9399,7 +9405,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/QCVMT/</v>
@@ -9427,7 +9433,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/QCVV/</v>
@@ -9455,7 +9461,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/QMAT/</v>
@@ -9483,7 +9489,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/QMTB/</v>
@@ -9511,7 +9517,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/QMTT/</v>
@@ -9539,7 +9545,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/QPMK/</v>
@@ -9567,7 +9573,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/QPMZ/</v>
@@ -9595,7 +9601,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/RESB/</v>
@@ -9623,7 +9629,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="str">
         <f>CONCATENATE(C112,D112,E112,F112,G112,H112,I112)</f>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/SAPAPO/</v>
@@ -9653,7 +9659,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="str">
         <f>CONCATENATE(C113,D113,E113,F113,G113,H113,I113)</f>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/SAPAPO/CHAR/MAT/</v>
@@ -9687,7 +9693,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="str">
         <f>CONCATENATE(C114,D114,E114,F114,G114,H114,I114)</f>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/SAPAPO/CHAR/MID/</v>
@@ -9721,7 +9727,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" t="str">
         <f>CONCATENATE(C115,D115,E115,F115,G115,H115)</f>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/STKO/</v>
@@ -9749,7 +9755,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/STPO/</v>
@@ -9777,7 +9783,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTM/TCRCOT/</v>
@@ -9805,7 +9811,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/A017/</v>
@@ -9833,7 +9839,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/A018/</v>
@@ -9861,7 +9867,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/EINA/</v>
@@ -9889,7 +9895,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/EINE/</v>
@@ -9917,7 +9923,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/EORD/</v>
@@ -9945,7 +9951,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/KNBK/</v>
@@ -9973,7 +9979,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/LFA1/</v>
@@ -10001,7 +10007,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/LFB1/</v>
@@ -10029,7 +10035,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/LFBK/</v>
@@ -10057,7 +10063,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/LFBW/</v>
@@ -10085,7 +10091,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/LFM1/</v>
@@ -10113,7 +10119,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/T001W/</v>
@@ -10141,7 +10147,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/T024E/</v>
@@ -10169,7 +10175,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/PTP/WYT3/</v>
@@ -10197,7 +10203,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/ANEP/</v>
@@ -10225,7 +10231,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/ANLA/</v>
@@ -10253,7 +10259,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/ANLB/</v>
@@ -10281,7 +10287,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/ANLC/</v>
@@ -10309,7 +10315,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" t="str">
         <f t="shared" si="8"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/ANLH/</v>
@@ -10337,13 +10343,13 @@
         <v>146</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" t="str">
-        <f t="shared" ref="A137:A194" si="12">CONCATENATE(C137,D137,E137,F137,G137,H137)</f>
+        <f t="shared" ref="A137:A196" si="12">CONCATENATE(C137,D137,E137,F137,G137,H137)</f>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/ANLZ/</v>
       </c>
       <c r="B137" t="str">
-        <f t="shared" ref="B137:B194" si="13">CONCATENATE(C137,K137,E137,F137,G137,H137)</f>
+        <f t="shared" ref="B137:B196" si="13">CONCATENATE(C137,K137,E137,F137,G137,H137)</f>
         <v>/SAPCO/Archive/MASTER_DATA_TABLES/RTR/ANLZ/</v>
       </c>
       <c r="C137" t="s">
@@ -10365,7 +10371,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/BKPF/</v>
@@ -10393,7 +10399,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/BNKA/</v>
@@ -10421,7 +10427,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/BSET/</v>
@@ -10449,7 +10455,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/BSIS/</v>
@@ -10477,7 +10483,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/CSKS/</v>
@@ -10505,7 +10511,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/CSKT/</v>
@@ -10533,7 +10539,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/PRHI/</v>
@@ -10561,7 +10567,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/PROJ/</v>
@@ -10589,7 +10595,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/PRPS/</v>
@@ -10617,7 +10623,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/SKA1/</v>
@@ -10645,7 +10651,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/SKAT/</v>
@@ -10673,7 +10679,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/SKB1/</v>
@@ -10701,7 +10707,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/ZBSEG/</v>
@@ -10729,7 +10735,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/RTR/ZBSIK/</v>
@@ -10757,7 +10763,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/AQUA/</v>
@@ -10785,7 +10791,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/BINMAT/</v>
@@ -10813,7 +10819,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/CONDINDX/</v>
@@ -10841,7 +10847,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/HUHDR/</v>
@@ -10869,7 +10875,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/LAGP/</v>
@@ -10897,7 +10903,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/MATLWH/</v>
@@ -10925,7 +10931,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/MATLWHST/</v>
@@ -10953,7 +10959,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/MCHA/</v>
@@ -10981,7 +10987,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/MKPF/</v>
@@ -11009,7 +11015,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/MSEG/</v>
@@ -11037,7 +11043,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/PAPAK/</v>
@@ -11065,7 +11071,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/PNPAKH/</v>
@@ -11093,7 +11099,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/PVPAKC/</v>
@@ -11121,7 +11127,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/PVPAKL/</v>
@@ -11149,7 +11155,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/QUAN/</v>
@@ -11177,7 +11183,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SAPAPO/MATLWH/</v>
@@ -11208,7 +11214,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" t="str">
         <f t="shared" ref="A168:A171" si="14">CONCATENATE(C168,D168,E168,F168,G168,H168)</f>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SAPAPO/MATLWHST/</v>
@@ -11239,7 +11245,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" t="str">
         <f t="shared" si="14"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SAPAPO/TR/</v>
@@ -11270,7 +11276,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" t="str">
         <f t="shared" si="14"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SAPAPO/TRM/</v>
@@ -11301,7 +11307,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" t="str">
         <f t="shared" si="14"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SAPAPO/TRMC/</v>
@@ -11332,13 +11338,13 @@
         <v>146</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" t="str">
-        <f t="shared" ref="A172" si="16">CONCATENATE(C172,D172,E172,F172,G172,H172)</f>
+        <f t="shared" ref="A172:A173" si="16">CONCATENATE(C172,D172,E172,F172,G172,H172)</f>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SAPAPO/TRMCARR/</v>
       </c>
       <c r="B172" t="str">
-        <f t="shared" ref="B172" si="17">CONCATENATE(C172,K172,E172,F172,G172,H172)</f>
+        <f t="shared" ref="B172:B173" si="17">CONCATENATE(C172,K172,E172,F172,G172,H172)</f>
         <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SAPAPO/TRMCARR/</v>
       </c>
       <c r="C172" t="s">
@@ -11363,14 +11369,14 @@
         <v>146</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" t="str">
-        <f t="shared" si="12"/>
-        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SAPCND/</v>
+        <f t="shared" si="16"/>
+        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SAPCN/</v>
       </c>
       <c r="B173" t="str">
-        <f t="shared" si="13"/>
-        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SAPCND/</v>
+        <f t="shared" si="17"/>
+        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SAPCN/</v>
       </c>
       <c r="C173" t="s">
         <v>211</v>
@@ -11385,20 +11391,21 @@
         <v>91</v>
       </c>
       <c r="G173" t="s">
-        <v>182</v>
-      </c>
+        <v>247</v>
+      </c>
+      <c r="H173" s="1"/>
       <c r="K173" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" t="str">
         <f t="shared" si="12"/>
-        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCMB/TOENTITY/</v>
+        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SAPCND/CONDINDX/</v>
       </c>
       <c r="B174" t="str">
         <f t="shared" si="13"/>
-        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCMB/TOENTITY/</v>
+        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SAPCND/CONDINDX/</v>
       </c>
       <c r="C174" t="s">
         <v>211</v>
@@ -11413,23 +11420,23 @@
         <v>91</v>
       </c>
       <c r="G174" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H174" s="1" t="s">
-        <v>238</v>
+        <v>169</v>
       </c>
       <c r="K174" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" t="str">
-        <f t="shared" ref="A175:A178" si="18">CONCATENATE(C175,D175,E175,F175,G175,H175)</f>
-        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCMB/ZONED/</v>
+        <f t="shared" ref="A175" si="18">CONCATENATE(C175,D175,E175,F175,G175,H175)</f>
+        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SAPCND/SAPCND_CONDINDX/</v>
       </c>
       <c r="B175" t="str">
-        <f t="shared" ref="B175:B178" si="19">CONCATENATE(C175,K175,E175,F175,G175,H175)</f>
-        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCMB/ZONED/</v>
+        <f t="shared" ref="B175" si="19">CONCATENATE(C175,K175,E175,F175,G175,H175)</f>
+        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SAPCND/SAPCND_CONDINDX/</v>
       </c>
       <c r="C175" t="s">
         <v>211</v>
@@ -11444,23 +11451,23 @@
         <v>91</v>
       </c>
       <c r="G175" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H175" s="1" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="K175" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" t="str">
-        <f t="shared" si="18"/>
-        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCMB/ZONEP/</v>
+        <f t="shared" si="12"/>
+        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCMB/TOENTITY/</v>
       </c>
       <c r="B176" t="str">
-        <f t="shared" si="19"/>
-        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCMB/ZONEP/</v>
+        <f t="shared" si="13"/>
+        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCMB/TOENTITY/</v>
       </c>
       <c r="C176" t="s">
         <v>211</v>
@@ -11478,20 +11485,20 @@
         <v>183</v>
       </c>
       <c r="H176" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K176" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" t="str">
-        <f t="shared" si="18"/>
-        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCMB/ZONER/</v>
+        <f t="shared" ref="A177:A180" si="20">CONCATENATE(C177,D177,E177,F177,G177,H177)</f>
+        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCMB/ZONED/</v>
       </c>
       <c r="B177" t="str">
-        <f t="shared" si="19"/>
-        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCMB/ZONER/</v>
+        <f t="shared" ref="B177:B180" si="21">CONCATENATE(C177,K177,E177,F177,G177,H177)</f>
+        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCMB/ZONED/</v>
       </c>
       <c r="C177" t="s">
         <v>211</v>
@@ -11509,20 +11516,20 @@
         <v>183</v>
       </c>
       <c r="H177" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K177" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" t="str">
-        <f t="shared" si="18"/>
-        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCMB/ZONE/</v>
+        <f t="shared" si="20"/>
+        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCMB/ZONEP/</v>
       </c>
       <c r="B178" t="str">
-        <f t="shared" si="19"/>
-        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCMB/ZONE/</v>
+        <f t="shared" si="21"/>
+        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCMB/ZONEP/</v>
       </c>
       <c r="C178" t="s">
         <v>211</v>
@@ -11540,83 +11547,83 @@
         <v>183</v>
       </c>
       <c r="H178" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="K178" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A179" t="str">
+        <f t="shared" si="20"/>
+        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCMB/ZONER/</v>
+      </c>
+      <c r="B179" t="str">
+        <f t="shared" si="21"/>
+        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCMB/ZONER/</v>
+      </c>
+      <c r="C179" t="s">
+        <v>211</v>
+      </c>
+      <c r="D179" t="s">
+        <v>3</v>
+      </c>
+      <c r="E179" t="s">
+        <v>27</v>
+      </c>
+      <c r="F179" t="s">
+        <v>91</v>
+      </c>
+      <c r="G179" t="s">
+        <v>183</v>
+      </c>
+      <c r="H179" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="K179" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A180" t="str">
+        <f t="shared" si="20"/>
+        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCMB/ZONE/</v>
+      </c>
+      <c r="B180" t="str">
+        <f t="shared" si="21"/>
+        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCMB/ZONE/</v>
+      </c>
+      <c r="C180" t="s">
+        <v>211</v>
+      </c>
+      <c r="D180" t="s">
+        <v>3</v>
+      </c>
+      <c r="E180" t="s">
+        <v>27</v>
+      </c>
+      <c r="F180" t="s">
+        <v>91</v>
+      </c>
+      <c r="G180" t="s">
+        <v>183</v>
+      </c>
+      <c r="H180" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="K178" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A179" t="str">
+      <c r="K180" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A181" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/AQUA/</v>
       </c>
-      <c r="B179" t="str">
+      <c r="B181" t="str">
         <f t="shared" si="13"/>
         <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCWM/AQUA/</v>
       </c>
-      <c r="C179" t="s">
-        <v>211</v>
-      </c>
-      <c r="D179" t="s">
-        <v>3</v>
-      </c>
-      <c r="E179" t="s">
-        <v>27</v>
-      </c>
-      <c r="F179" t="s">
-        <v>91</v>
-      </c>
-      <c r="G179" t="s">
-        <v>184</v>
-      </c>
-      <c r="H179" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="K179" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A180" t="str">
-        <f t="shared" ref="A180:A187" si="20">CONCATENATE(C180,D180,E180,F180,G180,H180)</f>
-        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/BINMAT/</v>
-      </c>
-      <c r="B180" t="str">
-        <f t="shared" ref="B180:B187" si="21">CONCATENATE(C180,K180,E180,F180,G180,H180)</f>
-        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCWM/BINMAT/</v>
-      </c>
-      <c r="C180" t="s">
-        <v>211</v>
-      </c>
-      <c r="D180" t="s">
-        <v>3</v>
-      </c>
-      <c r="E180" t="s">
-        <v>27</v>
-      </c>
-      <c r="F180" t="s">
-        <v>91</v>
-      </c>
-      <c r="G180" t="s">
-        <v>184</v>
-      </c>
-      <c r="H180" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="K180" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A181" t="str">
-        <f t="shared" si="20"/>
-        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/HUHDR/</v>
-      </c>
-      <c r="B181" t="str">
-        <f t="shared" si="21"/>
-        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCWM/HUHDR/</v>
-      </c>
       <c r="C181" t="s">
         <v>211</v>
       </c>
@@ -11633,20 +11640,20 @@
         <v>184</v>
       </c>
       <c r="H181" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K181" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" t="str">
-        <f t="shared" si="20"/>
-        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/LAGP/</v>
+        <f t="shared" ref="A182:A189" si="22">CONCATENATE(C182,D182,E182,F182,G182,H182)</f>
+        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/BINMAT/</v>
       </c>
       <c r="B182" t="str">
-        <f t="shared" si="21"/>
-        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCWM/LAGP/</v>
+        <f t="shared" ref="B182:B189" si="23">CONCATENATE(C182,K182,E182,F182,G182,H182)</f>
+        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCWM/BINMAT/</v>
       </c>
       <c r="C182" t="s">
         <v>211</v>
@@ -11664,20 +11671,20 @@
         <v>184</v>
       </c>
       <c r="H182" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="K182" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" t="str">
-        <f t="shared" si="20"/>
-        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/PAPAK/</v>
+        <f t="shared" si="22"/>
+        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/HUHDR/</v>
       </c>
       <c r="B183" t="str">
-        <f t="shared" si="21"/>
-        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCWM/PAPAK/</v>
+        <f t="shared" si="23"/>
+        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCWM/HUHDR/</v>
       </c>
       <c r="C183" t="s">
         <v>211</v>
@@ -11695,20 +11702,20 @@
         <v>184</v>
       </c>
       <c r="H183" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="K183" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" t="str">
-        <f t="shared" si="20"/>
-        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/PNPAKH/</v>
+        <f t="shared" si="22"/>
+        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/LAGP/</v>
       </c>
       <c r="B184" t="str">
-        <f t="shared" si="21"/>
-        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCWM/PNPAKH/</v>
+        <f t="shared" si="23"/>
+        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCWM/LAGP/</v>
       </c>
       <c r="C184" t="s">
         <v>211</v>
@@ -11726,20 +11733,20 @@
         <v>184</v>
       </c>
       <c r="H184" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="K184" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" t="str">
-        <f t="shared" si="20"/>
-        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/PVPAKC/</v>
+        <f t="shared" si="22"/>
+        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/PAPAK/</v>
       </c>
       <c r="B185" t="str">
-        <f t="shared" si="21"/>
-        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCWM/PVPAKC/</v>
+        <f t="shared" si="23"/>
+        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCWM/PAPAK/</v>
       </c>
       <c r="C185" t="s">
         <v>211</v>
@@ -11757,20 +11764,20 @@
         <v>184</v>
       </c>
       <c r="H185" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K185" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" t="str">
-        <f t="shared" si="20"/>
-        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/PVPAKL/</v>
+        <f t="shared" si="22"/>
+        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/PNPAKH/</v>
       </c>
       <c r="B186" t="str">
-        <f t="shared" si="21"/>
-        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCWM/PVPAKL/</v>
+        <f t="shared" si="23"/>
+        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCWM/PNPAKH/</v>
       </c>
       <c r="C186" t="s">
         <v>211</v>
@@ -11788,20 +11795,20 @@
         <v>184</v>
       </c>
       <c r="H186" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K186" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" t="str">
-        <f t="shared" si="20"/>
-        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/QUAN/</v>
+        <f t="shared" si="22"/>
+        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/PVPAKC/</v>
       </c>
       <c r="B187" t="str">
-        <f t="shared" si="21"/>
-        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCWM/QUAN/</v>
+        <f t="shared" si="23"/>
+        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCWM/PVPAKC/</v>
       </c>
       <c r="C187" t="s">
         <v>211</v>
@@ -11819,205 +11826,267 @@
         <v>184</v>
       </c>
       <c r="H187" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="K187" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A188" t="str">
+        <f t="shared" si="22"/>
+        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/PVPAKL/</v>
+      </c>
+      <c r="B188" t="str">
+        <f t="shared" si="23"/>
+        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCWM/PVPAKL/</v>
+      </c>
+      <c r="C188" t="s">
+        <v>211</v>
+      </c>
+      <c r="D188" t="s">
+        <v>3</v>
+      </c>
+      <c r="E188" t="s">
+        <v>27</v>
+      </c>
+      <c r="F188" t="s">
+        <v>91</v>
+      </c>
+      <c r="G188" t="s">
+        <v>184</v>
+      </c>
+      <c r="H188" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="K188" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A189" t="str">
+        <f t="shared" si="22"/>
+        <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/SCWM/QUAN/</v>
+      </c>
+      <c r="B189" t="str">
+        <f t="shared" si="23"/>
+        <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/SCWM/QUAN/</v>
+      </c>
+      <c r="C189" t="s">
+        <v>211</v>
+      </c>
+      <c r="D189" t="s">
+        <v>3</v>
+      </c>
+      <c r="E189" t="s">
+        <v>27</v>
+      </c>
+      <c r="F189" t="s">
+        <v>91</v>
+      </c>
+      <c r="G189" t="s">
+        <v>184</v>
+      </c>
+      <c r="H189" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="K187" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A188" t="str">
+      <c r="K189" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A190" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/T001L/</v>
       </c>
-      <c r="B188" t="str">
+      <c r="B190" t="str">
         <f t="shared" si="13"/>
         <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/T001L/</v>
       </c>
-      <c r="C188" t="s">
-        <v>211</v>
-      </c>
-      <c r="D188" t="s">
-        <v>3</v>
-      </c>
-      <c r="E188" t="s">
-        <v>27</v>
-      </c>
-      <c r="F188" t="s">
+      <c r="C190" t="s">
+        <v>211</v>
+      </c>
+      <c r="D190" t="s">
+        <v>3</v>
+      </c>
+      <c r="E190" t="s">
+        <v>27</v>
+      </c>
+      <c r="F190" t="s">
         <v>91</v>
       </c>
-      <c r="G188" t="s">
+      <c r="G190" t="s">
         <v>185</v>
       </c>
-      <c r="K188" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A189" t="str">
+      <c r="K190" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A191" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/TR/</v>
       </c>
-      <c r="B189" t="str">
+      <c r="B191" t="str">
         <f t="shared" si="13"/>
         <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/TR/</v>
       </c>
-      <c r="C189" t="s">
-        <v>211</v>
-      </c>
-      <c r="D189" t="s">
-        <v>3</v>
-      </c>
-      <c r="E189" t="s">
-        <v>27</v>
-      </c>
-      <c r="F189" t="s">
+      <c r="C191" t="s">
+        <v>211</v>
+      </c>
+      <c r="D191" t="s">
+        <v>3</v>
+      </c>
+      <c r="E191" t="s">
+        <v>27</v>
+      </c>
+      <c r="F191" t="s">
         <v>91</v>
       </c>
-      <c r="G189" t="s">
+      <c r="G191" t="s">
         <v>186</v>
       </c>
-      <c r="K189" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A190" t="str">
+      <c r="K191" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A192" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/TRM/</v>
       </c>
-      <c r="B190" t="str">
+      <c r="B192" t="str">
         <f t="shared" si="13"/>
         <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/TRM/</v>
       </c>
-      <c r="C190" t="s">
-        <v>211</v>
-      </c>
-      <c r="D190" t="s">
-        <v>3</v>
-      </c>
-      <c r="E190" t="s">
-        <v>27</v>
-      </c>
-      <c r="F190" t="s">
+      <c r="C192" t="s">
+        <v>211</v>
+      </c>
+      <c r="D192" t="s">
+        <v>3</v>
+      </c>
+      <c r="E192" t="s">
+        <v>27</v>
+      </c>
+      <c r="F192" t="s">
         <v>91</v>
       </c>
-      <c r="G190" t="s">
+      <c r="G192" t="s">
         <v>187</v>
       </c>
-      <c r="K190" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A191" t="str">
+      <c r="K192" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A193" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/TRMC/</v>
       </c>
-      <c r="B191" t="str">
+      <c r="B193" t="str">
         <f t="shared" si="13"/>
         <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/TRMC/</v>
       </c>
-      <c r="C191" t="s">
-        <v>211</v>
-      </c>
-      <c r="D191" t="s">
-        <v>3</v>
-      </c>
-      <c r="E191" t="s">
-        <v>27</v>
-      </c>
-      <c r="F191" t="s">
+      <c r="C193" t="s">
+        <v>211</v>
+      </c>
+      <c r="D193" t="s">
+        <v>3</v>
+      </c>
+      <c r="E193" t="s">
+        <v>27</v>
+      </c>
+      <c r="F193" t="s">
         <v>91</v>
       </c>
-      <c r="G191" t="s">
+      <c r="G193" t="s">
         <v>188</v>
       </c>
-      <c r="K191" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A192" t="str">
+      <c r="K193" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A194" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/TRMCARR/</v>
       </c>
-      <c r="B192" t="str">
+      <c r="B194" t="str">
         <f t="shared" si="13"/>
         <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/TRMCARR/</v>
       </c>
-      <c r="C192" t="s">
-        <v>211</v>
-      </c>
-      <c r="D192" t="s">
-        <v>3</v>
-      </c>
-      <c r="E192" t="s">
-        <v>27</v>
-      </c>
-      <c r="F192" t="s">
+      <c r="C194" t="s">
+        <v>211</v>
+      </c>
+      <c r="D194" t="s">
+        <v>3</v>
+      </c>
+      <c r="E194" t="s">
+        <v>27</v>
+      </c>
+      <c r="F194" t="s">
         <v>91</v>
       </c>
-      <c r="G192" t="s">
+      <c r="G194" t="s">
         <v>189</v>
       </c>
-      <c r="K192" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A193" t="str">
+      <c r="K194" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A195" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/SC/TVST</v>
       </c>
-      <c r="B193" t="str">
+      <c r="B195" t="str">
         <f t="shared" si="13"/>
         <v>/SAPCO/Archive/MASTER_DATA_TABLES/SC/TVST</v>
       </c>
-      <c r="C193" t="s">
-        <v>211</v>
-      </c>
-      <c r="D193" t="s">
-        <v>3</v>
-      </c>
-      <c r="E193" t="s">
-        <v>27</v>
-      </c>
-      <c r="F193" t="s">
+      <c r="C195" t="s">
+        <v>211</v>
+      </c>
+      <c r="D195" t="s">
+        <v>3</v>
+      </c>
+      <c r="E195" t="s">
+        <v>27</v>
+      </c>
+      <c r="F195" t="s">
         <v>91</v>
       </c>
-      <c r="G193" t="s">
+      <c r="G195" t="s">
         <v>190</v>
       </c>
-      <c r="K193" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A194" t="str">
+      <c r="K195" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A196" t="str">
         <f t="shared" si="12"/>
         <v>/SAPCO/Inbound/MASTER_DATA_TABLES/TEST/T001/</v>
       </c>
-      <c r="B194" t="str">
+      <c r="B196" t="str">
         <f t="shared" si="13"/>
         <v>/SAPCO/Archive/MASTER_DATA_TABLES/TEST/T001/</v>
       </c>
-      <c r="C194" t="s">
-        <v>211</v>
-      </c>
-      <c r="D194" t="s">
-        <v>3</v>
-      </c>
-      <c r="E194" t="s">
-        <v>27</v>
-      </c>
-      <c r="F194" t="s">
+      <c r="C196" t="s">
+        <v>211</v>
+      </c>
+      <c r="D196" t="s">
+        <v>3</v>
+      </c>
+      <c r="E196" t="s">
+        <v>27</v>
+      </c>
+      <c r="F196" t="s">
         <v>92</v>
       </c>
-      <c r="G194" t="s">
+      <c r="G196" t="s">
         <v>30</v>
       </c>
-      <c r="K194" t="s">
+      <c r="K196" t="s">
         <v>146</v>
       </c>
     </row>

</xml_diff>